<commit_message>
Partidos y 2 Creaciones
</commit_message>
<xml_diff>
--- a/ProcesosDesarrollados.xlsx
+++ b/ProcesosDesarrollados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krats\Documents\Git\Acceso-a-Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3730702-508C-48FF-A0C9-51688E0CB123}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587964B9-BAF7-4189-A9DB-3A5271D7A505}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>Proceso</t>
   </si>
@@ -94,7 +94,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,12 +131,6 @@
         <bgColor rgb="FF008000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor rgb="FF008000"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -151,7 +145,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -167,9 +161,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -587,7 +578,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +600,7 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -617,7 +608,7 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -633,7 +624,7 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -641,7 +632,7 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>